<commit_message>
update progress team plantenbak
</commit_message>
<xml_diff>
--- a/Log/Gantt Chart.xlsx
+++ b/Log/Gantt Chart.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/charlotte_bert_student_kuleuven_be/Documents/Sem 1/Project electronica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beauf\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{92D2890E-221C-4EA9-9C7A-3383D010F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AF44D0C-A0DA-49F7-84B5-6F8AEC45DBDB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2487F6F0-EBD6-45BA-B0F7-236BBC9233A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{616AC152-BF9F-4EFF-8CCF-DB0E2FE352C6}"/>
   </bookViews>
@@ -19,21 +19,10 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Online Gantt 20250218'!$A$1:$J$61</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -465,8 +454,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -494,9 +491,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -893,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9C8FD6-CA70-43F2-A589-F9B41CA79AEB}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,7 +946,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1">
@@ -1546,7 +1544,7 @@
       <c r="B22">
         <v>16</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D22" s="1">
@@ -1834,7 +1832,7 @@
       <c r="B31">
         <v>31</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D31" s="1">
@@ -1943,7 +1941,7 @@
         <v>61</v>
       </c>
       <c r="G34">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="H34" t="s">
         <v>23</v>
@@ -2039,7 +2037,7 @@
         <v>77</v>
       </c>
       <c r="G37">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H37" t="s">
         <v>12</v>
@@ -2071,7 +2069,7 @@
         <v>77</v>
       </c>
       <c r="G38">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H38" t="s">
         <v>12</v>
@@ -2186,7 +2184,7 @@
       <c r="B42">
         <v>46</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D42" s="1">

</xml_diff>